<commit_message>
Test fixes and address updates
</commit_message>
<xml_diff>
--- a/tests/test_files/usdm_excel_1.xlsx
+++ b/tests/test_files/usdm_excel_1.xlsx
@@ -12522,7 +12522,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>121 Seaport Boulevard||Boston|MA|02210|USA</t>
+          <t>121 Seaport Boulevard| |Boston|MA|02210|USA</t>
         </is>
       </c>
     </row>
@@ -12554,7 +12554,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>8600 Rockville Pike||Bethesda|MD|20894|USA</t>
+          <t>8600 Rockville Pike| |Bethesda|MD|20894|USA</t>
         </is>
       </c>
     </row>
@@ -12586,7 +12586,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Domenico Scarlattilaan 6||Amsterdam||1083 HS|NLD</t>
+          <t>Domenico Scarlattilaan 6| |Amsterdam| |1083 HS|NLD</t>
         </is>
       </c>
     </row>
@@ -12618,7 +12618,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>10903 New Hampshire Ave||Silver Spring|MD|20903|USA</t>
+          <t>10903 New Hampshire Ave| |Silver Spring|MD|20903|USA</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update for Arms and Epochs
</commit_message>
<xml_diff>
--- a/tests/test_files/usdm_excel_1.xlsx
+++ b/tests/test_files/usdm_excel_1.xlsx
@@ -12302,22 +12302,40 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>studyPhase</t>
+          <t>Epoch/Arms</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Phase II Trial</t>
+          <t>Screening</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Check In</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Treatment</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Follow-Up</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>spare</t>
+          <t>15mg-30mg</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -12433,10 +12451,6 @@
           <t>15mg-30mg</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>